<commit_message>
feat:64. Minimum Path Sum
</commit_message>
<xml_diff>
--- a/lc.xlsx
+++ b/lc.xlsx
@@ -5,14 +5,14 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ming/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ming/Documents/github/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="1220" yWindow="3160" windowWidth="22060" windowHeight="14840" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="工作表1" sheetId="1" r:id="rId1"/>
+    <sheet name="4" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>

</xml_diff>

<commit_message>
feat:442. Find All Duplicates in an Array
</commit_message>
<xml_diff>
--- a/lc.xlsx
+++ b/lc.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1220" yWindow="3160" windowWidth="22060" windowHeight="14840" tabRatio="500"/>
+    <workbookView xWindow="11560" yWindow="3160" windowWidth="22060" windowHeight="14840" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="4" sheetId="1" r:id="rId1"/>
+    <sheet name="442" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>index:</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -134,6 +135,26 @@
     <rPh sb="8" eb="9">
       <t>wei zhi</t>
     </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>null</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nums</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nums</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nums</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -184,7 +205,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -194,6 +215,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -474,8 +498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="G8:T23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -659,4 +683,220 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:J18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="6" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="9" width="6" style="4"/>
+    <col min="10" max="10" width="6" style="4" customWidth="1"/>
+    <col min="11" max="16384" width="6" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
+        <v>2</v>
+      </c>
+      <c r="F3" s="4">
+        <v>3</v>
+      </c>
+      <c r="G3" s="4">
+        <v>4</v>
+      </c>
+      <c r="H3" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4">
+        <v>3</v>
+      </c>
+      <c r="E4" s="4">
+        <v>4</v>
+      </c>
+      <c r="F4" s="4">
+        <v>5</v>
+      </c>
+      <c r="G4" s="4">
+        <v>5</v>
+      </c>
+      <c r="H4" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C5" s="4">
+        <v>-1</v>
+      </c>
+      <c r="F5" s="4">
+        <v>-5</v>
+      </c>
+      <c r="H5" s="4">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4">
+        <v>2</v>
+      </c>
+      <c r="F8" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C9" s="4">
+        <v>1</v>
+      </c>
+      <c r="D9" s="4">
+        <v>2</v>
+      </c>
+      <c r="E9" s="4">
+        <v>2</v>
+      </c>
+      <c r="F9" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C10" s="4">
+        <v>-1</v>
+      </c>
+      <c r="D10" s="4">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="4">
+        <v>1</v>
+      </c>
+      <c r="D13" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="4">
+        <v>-1</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1</v>
+      </c>
+      <c r="E16" s="4">
+        <v>2</v>
+      </c>
+      <c r="F16" s="4">
+        <v>3</v>
+      </c>
+      <c r="G16" s="4">
+        <v>4</v>
+      </c>
+      <c r="H16" s="4">
+        <v>5</v>
+      </c>
+      <c r="I16" s="4">
+        <v>6</v>
+      </c>
+      <c r="J16" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="C17" s="4">
+        <v>4</v>
+      </c>
+      <c r="D17" s="4">
+        <v>3</v>
+      </c>
+      <c r="E17" s="4">
+        <v>2</v>
+      </c>
+      <c r="F17" s="4">
+        <v>7</v>
+      </c>
+      <c r="G17" s="4">
+        <v>8</v>
+      </c>
+      <c r="H17" s="4">
+        <v>2</v>
+      </c>
+      <c r="I17" s="4">
+        <v>3</v>
+      </c>
+      <c r="J17" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B18" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="4">
+        <v>-3</v>
+      </c>
+      <c r="E18" s="4">
+        <v>-2</v>
+      </c>
+      <c r="F18" s="4">
+        <v>-7</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>